<commit_message>
Added visibility logic for rename and delete buttons in folderlistview in client side WPF2 project, also refactored method for enabling and disabling task details view controls in same project
</commit_message>
<xml_diff>
--- a/Client/TaskList2.UI.WPF2/Documentation/WPF2-UI-Element-Visibility-Map.xlsx
+++ b/Client/TaskList2.UI.WPF2/Documentation/WPF2-UI-Element-Visibility-Map.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Brian LeMaster\source\repos\TaskList2\Client\TaskList2.UI.WPF2\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{115897C8-5CA4-43AA-A38A-BC80DCA6D8A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A96143C1-7D3A-49B3-BE78-5DB46CB0DF1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="40920" yWindow="-120" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="1" xr2:uid="{E71A014A-C917-440C-A7AD-87C56019980A}"/>
   </bookViews>
@@ -40,6 +40,112 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Brian LeMaster</author>
+  </authors>
+  <commentList>
+    <comment ref="C1" authorId="0" shapeId="0" xr:uid="{118ECCE4-6C23-4CA0-BF4A-C08F094F8FF4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brian LeMaster:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Complete</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{28D683A8-26C6-4D7A-A42D-AEA5254E9696}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brian LeMaster:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Complete</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{5A04092C-CF69-4B65-A691-F77D4450C20D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brian LeMaster:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Complete</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{7B01F9B2-90EE-4E84-82FC-85869D143FDE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Brian LeMaster:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Complete</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="928" uniqueCount="51">
   <si>
@@ -200,7 +306,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,6 +443,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="10">
@@ -602,6 +721,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2476,24 +2599,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41F970F-8B63-46C6-9336-BC6DBEF4CBBA}">
-  <sheetPr filterMode="1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C41F970F-8B63-46C6-9336-BC6DBEF4CBBA}">
   <dimension ref="A1:O29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D3" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" activeCell="Q27" sqref="Q27"/>
+      <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="12.19921875" style="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.796875" style="14" customWidth="1"/>
-    <col min="3" max="3" width="15.86328125" style="14" hidden="1" customWidth="1"/>
-    <col min="4" max="14" width="15.86328125" style="14" customWidth="1"/>
-    <col min="15" max="15" width="15.86328125" style="14" hidden="1" customWidth="1"/>
+    <col min="3" max="15" width="15.86328125" style="14" customWidth="1"/>
     <col min="16" max="16384" width="9.06640625" style="14"/>
   </cols>
   <sheetData>
@@ -2544,7 +2664,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="42.75" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:15" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>38</v>
       </c>
@@ -3343,7 +3463,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A19" s="29" t="s">
         <v>24</v>
       </c>
@@ -3390,7 +3510,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A20" s="29" t="s">
         <v>24</v>
       </c>
@@ -3437,7 +3557,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A21" s="29" t="s">
         <v>24</v>
       </c>
@@ -3484,7 +3604,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A22" s="29" t="s">
         <v>19</v>
       </c>
@@ -3531,7 +3651,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A23" s="29" t="s">
         <v>19</v>
       </c>
@@ -3578,7 +3698,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A24" s="29" t="s">
         <v>25</v>
       </c>
@@ -3625,7 +3745,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A25" s="29" t="s">
         <v>25</v>
       </c>
@@ -3672,7 +3792,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A26" s="29" t="s">
         <v>25</v>
       </c>
@@ -3719,7 +3839,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A27" s="29" t="s">
         <v>25</v>
       </c>
@@ -3766,7 +3886,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A28" s="29" t="s">
         <v>25</v>
       </c>
@@ -3813,7 +3933,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:15" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A29" s="29" t="s">
         <v>25</v>
       </c>
@@ -3861,15 +3981,12 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:O29" xr:uid="{C41F970F-8B63-46C6-9336-BC6DBEF4CBBA}">
-    <filterColumn colId="13">
-      <colorFilter dxfId="0" cellColor="0"/>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:O29" xr:uid="{C41F970F-8B63-46C6-9336-BC6DBEF4CBBA}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O29">
     <sortCondition ref="D2:D29"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>